<commit_message>
First working example network.
</commit_message>
<xml_diff>
--- a/data/Kraftwerke_Lasten_Speichertabelle.xlsx
+++ b/data/Kraftwerke_Lasten_Speichertabelle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1F8428-4CDE-C049-BA60-876B6B363836}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E601E53D-18A1-F74B-8734-059A3E5B0D99}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="480" windowWidth="28240" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t xml:space="preserve"> Erlaube Vorgabe Bunkergröße oNB</t>
   </si>
   <si>
-    <t>Stellgröße xN in %</t>
-  </si>
-  <si>
     <t>Bunkergröße BN</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>Nachfüllrate nN in %</t>
+  </si>
+  <si>
+    <t>Stellgröße xN</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,10 +512,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -527,13 +527,13 @@
         <v>6</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="L1" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>7</v>
@@ -556,7 +556,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>0.2</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -567,7 +567,7 @@
       </c>
       <c r="H2">
         <f>5*E2</f>
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -593,27 +593,27 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>400</v>
+        <v>900</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G9" si="0">4*B3</f>
-        <v>1600</v>
+        <f t="shared" ref="G3:G10" si="0">4*B3</f>
+        <v>3600</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H9" si="1">5*E3</f>
-        <v>350</v>
+        <f t="shared" ref="H3:H10" si="1">5*E3</f>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -642,13 +642,13 @@
         <v>1300</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>0.2</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <v>0.2</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -659,7 +659,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -705,7 +705,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>40</v>
+        <v>-0.6</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -751,7 +751,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>-3</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -780,13 +780,13 @@
         <v>1000</v>
       </c>
       <c r="C7">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>0.7</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -797,7 +797,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>3.5</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -832,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -843,7 +843,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>-5</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -910,10 +910,97 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>700</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>25000</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11" si="2">4*B11</f>
+        <v>100000</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11" si="3">5*E11</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I13" s="3"/>

</xml_diff>

<commit_message>
Wetterdaten den Kraftwerken zuordnen
</commit_message>
<xml_diff>
--- a/data/Kraftwerke_Lasten_Speichertabelle.xlsx
+++ b/data/Kraftwerke_Lasten_Speichertabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DE1D0D-44FC-7B4D-B9B2-22E674A51530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C357A1DF-379F-B846-AD0B-62626C2505E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="440" windowWidth="28240" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="28240" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nennleistung PN</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Netzverknüpfungspunkt K</t>
+  </si>
+  <si>
+    <t>Trendquelle</t>
+  </si>
+  <si>
+    <t>weather/wind/Goteborg_Juli_2019.json</t>
+  </si>
+  <si>
+    <t>weather/wind/Muenchen_Juli_2019.json</t>
+  </si>
+  <si>
+    <t>weather/wind/Bremerhaven_Juli_2019.json</t>
   </si>
 </sst>
 </file>
@@ -483,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,6 +516,7 @@
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="25.83203125" customWidth="1"/>
     <col min="15" max="15" width="30.1640625" customWidth="1"/>
+    <col min="16" max="16" width="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -552,6 +565,9 @@
       <c r="O1" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -584,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -633,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -682,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -731,7 +747,7 @@
         <v>-3</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -780,7 +796,7 @@
         <v>3.5</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -927,7 +943,7 @@
         <v>-5</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -968,15 +984,15 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10" si="2">4*C10</f>
+        <f t="shared" ref="H10:H13" si="2">4*C10</f>
         <v>100000</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10" si="3">5*F10</f>
+        <f t="shared" ref="I10:I13" si="3">5*F10</f>
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -994,20 +1010,167 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P16" s="5"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>

</xml_diff>

<commit_message>
Speicher mit vollem oder leerem Bunker nicht überfahren.
</commit_message>
<xml_diff>
--- a/data/Kraftwerke_Lasten_Speichertabelle.xlsx
+++ b/data/Kraftwerke_Lasten_Speichertabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B681843-309D-ED40-A4C3-9F68C373F8F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B0EE7A-2221-654B-9907-37CF48E5CC66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16260" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,14 +121,6 @@
       <color theme="1"/>
       <name val="Courier"/>
       <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,10 +173,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -193,6 +184,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -510,7 +502,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +517,7 @@
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="25.83203125" customWidth="1"/>
@@ -534,52 +526,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -692,7 +684,7 @@
         <v>300</v>
       </c>
       <c r="D4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -718,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -744,13 +736,13 @@
         <v>-1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>-0.6</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -767,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -790,10 +782,10 @@
         <v>1000</v>
       </c>
       <c r="D6">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="E6">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0.7</v>
@@ -865,7 +857,7 @@
         <v>3000</v>
       </c>
       <c r="L7">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="M7">
         <v>-2</v>
@@ -914,7 +906,7 @@
         <v>1700</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M8">
         <v>-1</v>
@@ -1057,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1104,22 +1096,22 @@
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12" s="3">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3">
-        <v>0</v>
-      </c>
-      <c r="N12" s="3">
-        <v>0</v>
-      </c>
-      <c r="O12" s="3">
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
@@ -1225,86 +1217,86 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14" s="5"/>
+      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P15" s="5"/>
+      <c r="P15" s="4"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="Q19" s="2"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="H22" s="9"/>
-      <c r="I22" s="11"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="12"/>
-      <c r="C23" s="10"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="7"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="9"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C25" s="8"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C26" s="8"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="6"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C27" s="8"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="6"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C28" s="8"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="6"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C29" s="8"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C30" s="8"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="6"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C31" s="7"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" s="7"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+      <c r="C36" s="6"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integration von profilgesteuerten Lasten
</commit_message>
<xml_diff>
--- a/data/Kraftwerke_Lasten_Speichertabelle.xlsx
+++ b/data/Kraftwerke_Lasten_Speichertabelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B0EE7A-2221-654B-9907-37CF48E5CC66}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E22A8A-EFE3-F34C-800A-05F131A59B11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16260" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nennleistung PN</t>
   </si>
@@ -81,13 +81,13 @@
     <t>Trendquelle</t>
   </si>
   <si>
+    <t>weather/wind/Muenchen_Juli_2019.json</t>
+  </si>
+  <si>
+    <t>load/city/last_4_7_2019.xlsx</t>
+  </si>
+  <si>
     <t>weather/wind/Goteborg_Juli_2019.json</t>
-  </si>
-  <si>
-    <t>weather/wind/Muenchen_Juli_2019.json</t>
-  </si>
-  <si>
-    <t>weather/wind/Bremerhaven_Juli_2019.json</t>
   </si>
 </sst>
 </file>
@@ -169,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -184,7 +184,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -499,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +524,7 @@
     <col min="16" max="16" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -575,7 +574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -598,11 +597,11 @@
         <v>2</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H9" si="0">4*C2</f>
+        <f t="shared" ref="H2:H7" si="0">4*C2</f>
         <v>3600</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I9" si="1">5*F2</f>
+        <f t="shared" ref="I2:I7" si="1">5*F2</f>
         <v>0</v>
       </c>
       <c r="J2">
@@ -624,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -635,7 +634,7 @@
         <v>1300</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <v>-1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -673,7 +672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -722,7 +721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -771,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -820,133 +819,132 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>700</v>
       </c>
       <c r="D7">
         <v>-1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F7">
         <v>-1</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>2800</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>90</v>
+        <v>25000</v>
       </c>
       <c r="D8">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>360</v>
+        <f t="shared" ref="H8:H12" si="2">4*C8</f>
+        <v>100000</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" ref="I8:I12" si="3">5*F8</f>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M8">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="D9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>2800</v>
+        <f t="shared" si="2"/>
+        <v>400</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -966,16 +964,19 @@
       <c r="O9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>25000</v>
+        <v>500</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -987,15 +988,13 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H10:H14" si="2">4*C10</f>
-        <v>100000</v>
+        <v>2000</v>
       </c>
       <c r="I10">
-        <f t="shared" ref="I10:I14" si="3">5*F10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1015,35 +1014,39 @@
       <c r="O10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
         <v>400</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>-5</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1063,89 +1066,89 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
         <v>4</v>
-      </c>
-      <c r="C12">
-        <v>200</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="12">
-        <v>0</v>
-      </c>
-      <c r="O12" s="12">
+        <f t="shared" si="3"/>
+        <v>-5</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>2000</v>
+        <f t="shared" ref="H13" si="4">4*C13</f>
+        <v>1200</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <f t="shared" ref="I13" si="5">5*F13</f>
+        <v>-5</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1166,134 +1169,81 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>-1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>400</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
-        <v>-5</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P15" s="4"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H19" s="8"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="7"/>
       <c r="H22" s="8"/>
       <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="11"/>
-      <c r="C23" s="9"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="7"/>
       <c r="H23" s="8"/>
       <c r="I23" s="10"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C24" s="7"/>
       <c r="H24" s="8"/>
       <c r="I24" s="10"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C25" s="7"/>
       <c r="H25" s="8"/>
       <c r="I25" s="10"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C26" s="7"/>
-      <c r="H26" s="8"/>
       <c r="I26" s="10"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C27" s="7"/>
-      <c r="H27" s="8"/>
       <c r="I27" s="10"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C28" s="7"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C29" s="7"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C30" s="7"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C31" s="6"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" s="6"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C28" s="6"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="6"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Kostenfunktionen entworfen, Abbruch der Berechnung bei nicht regelbarem Netz.
</commit_message>
<xml_diff>
--- a/data/Kraftwerke_Lasten_Speichertabelle.xlsx
+++ b/data/Kraftwerke_Lasten_Speichertabelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lars/Documents/MATLAB/Netzsimulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E22A8A-EFE3-F34C-800A-05F131A59B11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417B4D75-5881-264A-9E32-A3CDBAEF53D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16240" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{109839D1-D567-AA4B-87D7-F86B2B8F67E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,21 +33,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
-    <t>Nennleistung PN</t>
-  </si>
-  <si>
     <t>xNmin</t>
   </si>
   <si>
     <t>xNmax</t>
   </si>
   <si>
-    <t>Fixkosten CN</t>
-  </si>
-  <si>
-    <t>variable Kosten cN</t>
-  </si>
-  <si>
     <t>Erlaubnis Vorgabe Nennleistung oNP</t>
   </si>
   <si>
@@ -57,9 +48,6 @@
     <t xml:space="preserve"> Erlaube Vorgabe Bunkergröße oNB</t>
   </si>
   <si>
-    <t>Bunkergröße BN</t>
-  </si>
-  <si>
     <t>Bunkerfüllstand bN</t>
   </si>
   <si>
@@ -88,6 +76,18 @@
   </si>
   <si>
     <t>weather/wind/Goteborg_Juli_2019.json</t>
+  </si>
+  <si>
+    <t>Fixkosten CN [€/Jahr]</t>
+  </si>
+  <si>
+    <t>variable Kosten cN [€/kWh]</t>
+  </si>
+  <si>
+    <t>Nennleistung PN [kW]</t>
+  </si>
+  <si>
+    <t>Bunkergröße BN [kWh]</t>
   </si>
 </sst>
 </file>
@@ -500,23 +500,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660CDFC1-36C3-6D4A-97C5-40145D00575F}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" customWidth="1"/>
     <col min="7" max="7" width="57.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
     <col min="12" max="12" width="17.1640625" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="25.83203125" customWidth="1"/>
@@ -526,52 +526,52 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="O1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -582,27 +582,26 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>900</v>
+        <v>900000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H7" si="0">4*C2</f>
-        <v>3600</v>
+        <f>4000000000/40</f>
+        <v>100000000</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I7" si="1">5*F2</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -631,27 +630,26 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1300</v>
+        <v>1400000</v>
       </c>
       <c r="D3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
-        <v>5200</v>
+        <f>1000000000/40</f>
+        <v>25000000</v>
       </c>
       <c r="I3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.13</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -680,10 +678,10 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>300</v>
+        <v>16400</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -694,19 +692,18 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>1200</v>
+      <c r="H4" s="8">
+        <v>1230000</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>H4*20*0.25/(1000*K4)</f>
+        <v>0.246</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="L4">
         <v>0.5</v>
@@ -729,33 +726,33 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>500</v>
+        <v>22000</v>
       </c>
       <c r="D5">
         <v>-1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>-0.6</v>
+        <v>-1</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
-        <v>2000</v>
+        <f>17000000/20</f>
+        <v>850000</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
-        <v>-3</v>
+        <f>H5*20*0.25/(1000*K5)</f>
+        <v>0.25757575757575757</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>16500</v>
       </c>
       <c r="L5">
         <v>0.5</v>
@@ -778,7 +775,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>1000</v>
+        <v>1600000</v>
       </c>
       <c r="D6">
         <v>0.2</v>
@@ -787,18 +784,17 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
-        <v>4000</v>
+        <f>2000000000/40</f>
+        <v>50000000</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>0.05</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -827,7 +823,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>700</v>
+        <v>700000</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -842,12 +838,10 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -876,7 +870,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>25000</v>
+        <v>2000000</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -891,12 +885,11 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H12" si="2">4*C8</f>
-        <v>100000</v>
+        <f>1000000000/40</f>
+        <v>25000000</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I12" si="3">5*F8</f>
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -925,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -934,17 +927,17 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
-        <v>400</v>
+        <f>C9*1000/20</f>
+        <v>5000000</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -965,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -976,7 +969,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>500</v>
+        <v>500000</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -991,10 +984,11 @@
         <v>3</v>
       </c>
       <c r="H10">
-        <v>2000</v>
+        <f>C10*1000/20</f>
+        <v>25000000</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1015,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1026,7 +1020,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -1041,12 +1035,10 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1076,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -1091,12 +1083,10 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1117,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -1128,7 +1118,7 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>300</v>
+        <v>300000</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -1143,12 +1133,10 @@
         <v>4</v>
       </c>
       <c r="H13">
-        <f t="shared" ref="H13" si="4">4*C13</f>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13" si="5">5*F13</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1169,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1241,7 +1229,6 @@
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C33" s="6"/>
-      <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>

</xml_diff>